<commit_message>
updated mongolia to include latest data
</commit_message>
<xml_diff>
--- a/mongolia/transformations/templates/calibrated/mongolia/model_input_variables_mongolia_ce_calibrated.xlsx
+++ b/mongolia/transformations/templates/calibrated/mongolia/model_input_variables_mongolia_ce_calibrated.xlsx
@@ -14155,7 +14155,7 @@
         <v>117</v>
       </c>
       <c r="C107">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H107">
         <v>1</v>
@@ -14280,7 +14280,7 @@
         <v>118</v>
       </c>
       <c r="C108">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -14405,7 +14405,7 @@
         <v>119</v>
       </c>
       <c r="C109">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -14530,7 +14530,7 @@
         <v>120</v>
       </c>
       <c r="C110">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -14655,7 +14655,7 @@
         <v>121</v>
       </c>
       <c r="C111">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -14780,7 +14780,7 @@
         <v>122</v>
       </c>
       <c r="C112">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -14905,7 +14905,7 @@
         <v>123</v>
       </c>
       <c r="C113">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -15030,7 +15030,7 @@
         <v>124</v>
       </c>
       <c r="C114">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -15155,7 +15155,7 @@
         <v>125</v>
       </c>
       <c r="C115">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H115">
         <v>1</v>
@@ -15280,7 +15280,7 @@
         <v>126</v>
       </c>
       <c r="C116">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H116">
         <v>1</v>
@@ -15405,7 +15405,7 @@
         <v>127</v>
       </c>
       <c r="C117">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H117">
         <v>1</v>
@@ -15530,7 +15530,7 @@
         <v>128</v>
       </c>
       <c r="C118">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -15655,7 +15655,7 @@
         <v>129</v>
       </c>
       <c r="C119">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H119">
         <v>1</v>
@@ -15780,7 +15780,7 @@
         <v>130</v>
       </c>
       <c r="C120">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H120">
         <v>1</v>
@@ -15905,7 +15905,7 @@
         <v>131</v>
       </c>
       <c r="C121">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H121">
         <v>1</v>
@@ -16030,7 +16030,7 @@
         <v>132</v>
       </c>
       <c r="C122">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H122">
         <v>1</v>
@@ -16155,7 +16155,7 @@
         <v>133</v>
       </c>
       <c r="C123">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H123">
         <v>1</v>
@@ -16280,7 +16280,7 @@
         <v>134</v>
       </c>
       <c r="C124">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -16405,7 +16405,7 @@
         <v>135</v>
       </c>
       <c r="C125">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -16530,7 +16530,7 @@
         <v>136</v>
       </c>
       <c r="C126">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H126">
         <v>1</v>
@@ -16655,7 +16655,7 @@
         <v>137</v>
       </c>
       <c r="C127">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H127">
         <v>1</v>
@@ -16780,7 +16780,7 @@
         <v>138</v>
       </c>
       <c r="C128">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H128">
         <v>1</v>
@@ -16905,7 +16905,7 @@
         <v>139</v>
       </c>
       <c r="C129">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H129">
         <v>1</v>
@@ -17030,7 +17030,7 @@
         <v>140</v>
       </c>
       <c r="C130">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H130">
         <v>1</v>
@@ -17155,7 +17155,7 @@
         <v>141</v>
       </c>
       <c r="C131">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -17280,7 +17280,7 @@
         <v>142</v>
       </c>
       <c r="C132">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H132">
         <v>1</v>

</xml_diff>

<commit_message>
added strategy templates for mongolia
</commit_message>
<xml_diff>
--- a/mongolia/transformations/templates/calibrated/mongolia/model_input_variables_mongolia_ce_calibrated.xlsx
+++ b/mongolia/transformations/templates/calibrated/mongolia/model_input_variables_mongolia_ce_calibrated.xlsx
@@ -14155,7 +14155,7 @@
         <v>117</v>
       </c>
       <c r="C107">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H107">
         <v>1</v>
@@ -14280,7 +14280,7 @@
         <v>118</v>
       </c>
       <c r="C108">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -14405,7 +14405,7 @@
         <v>119</v>
       </c>
       <c r="C109">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -14530,7 +14530,7 @@
         <v>120</v>
       </c>
       <c r="C110">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -14655,7 +14655,7 @@
         <v>121</v>
       </c>
       <c r="C111">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -14780,7 +14780,7 @@
         <v>122</v>
       </c>
       <c r="C112">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H112">
         <v>1</v>
@@ -14905,7 +14905,7 @@
         <v>123</v>
       </c>
       <c r="C113">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -15030,7 +15030,7 @@
         <v>124</v>
       </c>
       <c r="C114">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -15155,7 +15155,7 @@
         <v>125</v>
       </c>
       <c r="C115">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H115">
         <v>1</v>
@@ -15280,7 +15280,7 @@
         <v>126</v>
       </c>
       <c r="C116">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H116">
         <v>1</v>
@@ -15405,7 +15405,7 @@
         <v>127</v>
       </c>
       <c r="C117">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H117">
         <v>1</v>
@@ -15530,7 +15530,7 @@
         <v>128</v>
       </c>
       <c r="C118">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -15655,7 +15655,7 @@
         <v>129</v>
       </c>
       <c r="C119">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="H119">
         <v>1</v>
@@ -15780,7 +15780,7 @@
         <v>130</v>
       </c>
       <c r="C120">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H120">
         <v>1</v>
@@ -15905,7 +15905,7 @@
         <v>131</v>
       </c>
       <c r="C121">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H121">
         <v>1</v>
@@ -16030,7 +16030,7 @@
         <v>132</v>
       </c>
       <c r="C122">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H122">
         <v>1</v>
@@ -16155,7 +16155,7 @@
         <v>133</v>
       </c>
       <c r="C123">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H123">
         <v>1</v>
@@ -16280,7 +16280,7 @@
         <v>134</v>
       </c>
       <c r="C124">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H124">
         <v>1</v>
@@ -16405,7 +16405,7 @@
         <v>135</v>
       </c>
       <c r="C125">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H125">
         <v>1</v>
@@ -16530,7 +16530,7 @@
         <v>136</v>
       </c>
       <c r="C126">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H126">
         <v>1</v>
@@ -16655,7 +16655,7 @@
         <v>137</v>
       </c>
       <c r="C127">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H127">
         <v>1</v>
@@ -16780,7 +16780,7 @@
         <v>138</v>
       </c>
       <c r="C128">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H128">
         <v>1</v>
@@ -16905,7 +16905,7 @@
         <v>139</v>
       </c>
       <c r="C129">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H129">
         <v>1</v>
@@ -17030,7 +17030,7 @@
         <v>140</v>
       </c>
       <c r="C130">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H130">
         <v>1</v>
@@ -17155,7 +17155,7 @@
         <v>141</v>
       </c>
       <c r="C131">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -17280,7 +17280,7 @@
         <v>142</v>
       </c>
       <c r="C132">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H132">
         <v>1</v>

</xml_diff>